<commit_message>
new basis is not A-1e as vectors AL=A-1X but Ae instead
</commit_message>
<xml_diff>
--- a/math/tools_docs/linear_forms.xlsx
+++ b/math/tools_docs/linear_forms.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>F</t>
   </si>
@@ -151,6 +151,21 @@
   </si>
   <si>
     <t>A-1</t>
+  </si>
+  <si>
+    <t>A-1e1</t>
+  </si>
+  <si>
+    <t>A-1e2</t>
+  </si>
+  <si>
+    <t>This is not correct...</t>
+  </si>
+  <si>
+    <t>This is correct</t>
+  </si>
+  <si>
+    <t>=A-1X</t>
   </si>
 </sst>
 </file>
@@ -173,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +207,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -205,12 +244,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +558,7 @@
   <dimension ref="D4:AA47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,21 +597,21 @@
         <v>1</v>
       </c>
       <c r="J6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6" t="s">
         <v>1</v>
       </c>
       <c r="O6">
         <f t="array" ref="O6:O7">MMULT(I6:J7,E6:E7)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R6" t="s">
         <v>2</v>
       </c>
       <c r="S6" s="4">
         <f t="array" ref="S6">MMULT(TRANSPOSE(E6:E7),O6:O7)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="X6" t="s">
         <v>42</v>
@@ -581,7 +624,7 @@
       </c>
       <c r="AA6">
         <f t="array" ref="AA6">MMULT(TRANSPOSE(Y4:Y5),MMULT(I6:J7,Y6:Y7))</f>
-        <v>-4</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="7" spans="4:27" x14ac:dyDescent="0.25">
@@ -589,13 +632,13 @@
         <v>1</v>
       </c>
       <c r="I7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Y7">
         <v>-3</v>
@@ -607,7 +650,7 @@
       </c>
       <c r="E10">
         <f t="array" ref="E10:E11">MMULT(MINVERSE(I14:J15),E6:E7)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H10" t="s">
         <v>3</v>
@@ -624,14 +667,14 @@
       </c>
       <c r="O10">
         <f t="array" ref="O10:O11">MMULT(I10:J11,E10:E11)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R10" t="s">
         <v>8</v>
       </c>
       <c r="S10">
         <f t="array" ref="S10">MMULT(TRANSPOSE(E10:E11),O10:O11)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="4:27" x14ac:dyDescent="0.25">
@@ -646,10 +689,10 @@
       </c>
       <c r="J11">
         <f>-(I7^2)/I6+J7</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="4:27" x14ac:dyDescent="0.25">
@@ -666,7 +709,7 @@
       </c>
       <c r="J14">
         <f>-I7/I6</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="15" spans="4:27" x14ac:dyDescent="0.25">
@@ -689,12 +732,12 @@
       <c r="D19" t="s">
         <v>13</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="E20">
+      <c r="E20" s="5">
         <v>0</v>
       </c>
     </row>
@@ -702,16 +745,22 @@
       <c r="D21" t="s">
         <v>14</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="E22">
+      <c r="E22" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" t="s">
+        <v>47</v>
+      </c>
       <c r="O24" t="s">
         <v>35</v>
       </c>
@@ -720,7 +769,7 @@
       <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="8">
         <v>1</v>
       </c>
       <c r="G25" t="s">
@@ -730,31 +779,45 @@
         <f t="array" ref="H25:H26">MMULT(I14:J15,E19:E20)</f>
         <v>1</v>
       </c>
-      <c r="O25" t="s">
+      <c r="J25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25">
+        <f t="array" ref="K25:K26">MMULT(R43:S44,E19:E20)</f>
+        <v>1</v>
+      </c>
+      <c r="O25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="R25" t="s">
+      <c r="P25" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="5">
         <f>-I7/I6</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="26" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="E26">
+      <c r="E26" s="8">
         <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="S26">
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5">
         <v>1</v>
       </c>
     </row>
@@ -762,22 +825,32 @@
       <c r="D28" t="s">
         <v>10</v>
       </c>
-      <c r="E28">
-        <v>-1</v>
+      <c r="E28" s="7">
+        <v>-2</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
       </c>
       <c r="H28">
         <f t="array" ref="H28:H29">MMULT(I14:J15,E21:E22)</f>
-        <v>-1</v>
+        <v>-2</v>
+      </c>
+      <c r="J28" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28">
+        <f t="array" ref="K28:K29">MMULT(R43:S44,E21:E22)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="E29">
+      <c r="E29" s="7">
         <v>1</v>
       </c>
       <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="K29">
         <v>1</v>
       </c>
     </row>
@@ -845,7 +918,7 @@
       </c>
       <c r="S36" s="3">
         <f>M42</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="V36" t="s">
         <v>26</v>
@@ -876,10 +949,10 @@
         <v>1</v>
       </c>
       <c r="W37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X37">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="39" spans="4:26" x14ac:dyDescent="0.25">
@@ -903,7 +976,7 @@
       </c>
       <c r="R39">
         <f t="array" ref="R39:R40">MMULT(MINVERSE(R36:S37),E6:E7)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U39" s="3" t="s">
         <v>37</v>
@@ -926,6 +999,9 @@
       <c r="D40" t="s">
         <v>21</v>
       </c>
+      <c r="Q40" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="R40">
         <v>1</v>
       </c>
@@ -933,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="X40" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z40" t="s">
         <v>33</v>
@@ -947,7 +1023,7 @@
     <row r="42" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D42">
         <f>E28</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="E42">
         <f>E29</f>
@@ -972,7 +1048,7 @@
       </c>
       <c r="M42">
         <f t="array" ref="M42:N42">MMULT(D42:E42,MINVERSE(H42:I43))</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="N42">
         <v>1</v>
@@ -995,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="S43" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="4:26" x14ac:dyDescent="0.25">
@@ -1010,7 +1086,7 @@
       </c>
       <c r="W44" s="4">
         <f t="array" ref="W44">MMULT(TRANSPOSE(R39:R40),MMULT(W39:X40,R39:R40))</f>
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="4:26" x14ac:dyDescent="0.25">
@@ -1027,7 +1103,7 @@
       </c>
       <c r="X47" s="4">
         <f>(R39^2)*W39+(R40^2)*X40</f>
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>